<commit_message>
Prognose, Erstellung des Grundgerüstes der Module
</commit_message>
<xml_diff>
--- a/docs/PrognoseCalc/PrognoseCalc-ABSCalc.xlsx
+++ b/docs/PrognoseCalc/PrognoseCalc-ABSCalc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smailthkoelnde-my.sharepoint.com/personal/thomas_schumann_smailthkoelnde_onmicrosoft_com/Documents/Dokumente/01_TH Köln/08_GdW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\thoma\IdeaProjects\GDWWS2021GeraschSalamonSchumann\docs\PrognoseCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="552" documentId="8_{1EC803AC-6612-486A-A5CF-53856FDFB813}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{36E1A79B-5B08-4926-98BE-698BB2018A01}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB19689-ECCE-4DE6-BB86-224804856500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27960" yWindow="765" windowWidth="27450" windowHeight="18840" tabRatio="857" activeTab="5" xr2:uid="{6A5BFC6A-5A01-4EA7-8DAE-9EDEA8B95B90}"/>
+    <workbookView xWindow="-29580" yWindow="1215" windowWidth="27450" windowHeight="18840" tabRatio="857" activeTab="5" xr2:uid="{6A5BFC6A-5A01-4EA7-8DAE-9EDEA8B95B90}"/>
   </bookViews>
   <sheets>
     <sheet name="05374-OBK2021" sheetId="1" r:id="rId1"/>
@@ -326,14 +326,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -343,13 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -669,7 +669,7 @@
   <dimension ref="A2:V30"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E30" sqref="E30:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,24 +686,24 @@
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="18"/>
       <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
@@ -899,44 +899,44 @@
       </c>
     </row>
     <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
-        <v>0</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12" t="s">
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
         <v>7</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>14</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>38</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <v>72</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>18</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <v>48</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="10">
         <v>44</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11">
+      <c r="N9" s="10"/>
+      <c r="O9" s="10">
         <f t="shared" si="0"/>
         <v>241</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="10">
         <f t="shared" si="1"/>
         <v>88.595775341700303</v>
       </c>
@@ -1191,99 +1191,93 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-      <c r="I27" s="13" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="I27" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="15"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16">
+      <c r="B28" s="12">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>131.91111111111113</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="I28" s="16">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="I28" s="12">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>48.492809813585417</v>
       </c>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="18"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="14"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="13" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
-      <c r="I29" s="13" t="s">
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="I29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="14"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="13" t="s">
+      <c r="J29" s="16"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="14"/>
-      <c r="N29" s="15"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16">
+      <c r="B30" s="12">
         <f>O10</f>
         <v>128</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="16">
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="12">
         <f>B28-B30</f>
         <v>3.9111111111111256</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="I30" s="16">
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="I30" s="12">
         <f>P10</f>
         <v>47.055017608869875</v>
       </c>
-      <c r="J30" s="17"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="16">
+      <c r="J30" s="13"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="12">
         <f>I28-I30</f>
         <v>1.4377922047155423</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="18"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="L29:N29"/>
     <mergeCell ref="G3:M3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="B30:D30"/>
@@ -1292,6 +1286,12 @@
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="I27:N27"/>
     <mergeCell ref="I28:N28"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="L29:N29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1304,7 +1304,7 @@
   <dimension ref="A2:P30"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E30" sqref="E30:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,24 +1321,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="18"/>
       <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1528,44 +1528,44 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
-        <v>0</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12" t="s">
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
         <v>8</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>48</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>40</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <v>45</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>21</v>
       </c>
-      <c r="L9" s="11">
-        <v>0</v>
-      </c>
-      <c r="M9" s="11">
+      <c r="L9" s="10">
+        <v>0</v>
+      </c>
+      <c r="M9" s="10">
         <v>3</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11">
+      <c r="N9" s="10"/>
+      <c r="O9" s="10">
         <f t="shared" si="0"/>
         <v>165</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="10">
         <f t="shared" si="1"/>
         <v>15.988372093023255</v>
       </c>
@@ -1826,90 +1826,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-      <c r="I27" s="13" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="I27" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="15"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16">
+      <c r="B28" s="12">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>48.533333333333339</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="I28" s="16">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="I28" s="12">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>4.7028423772609891</v>
       </c>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="18"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="14"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="13" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
-      <c r="I29" s="13" t="s">
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="I29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="14"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="13" t="s">
+      <c r="J29" s="16"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="14"/>
-      <c r="N29" s="15"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16">
+      <c r="B30" s="12">
         <f>O10</f>
         <v>122</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="16">
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="12">
         <f>B28-B30</f>
         <v>-73.466666666666669</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="I30" s="16">
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="I30" s="12">
         <f>P10</f>
         <v>11.821705426356589</v>
       </c>
-      <c r="J30" s="17"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="16">
+      <c r="J30" s="13"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="12">
         <f>I28-I30</f>
         <v>-7.1188630490955997</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="18"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1938,7 +1938,7 @@
   <dimension ref="A2:P30"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:N21"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,24 +1955,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="18"/>
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
@@ -2162,44 +2162,44 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
-        <v>0</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12" t="s">
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
         <v>70</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>96</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>81</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <v>74</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>77</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <v>26</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="10">
         <v>12</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11">
+      <c r="N9" s="10"/>
+      <c r="O9" s="10">
         <f t="shared" si="0"/>
         <v>436</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="10">
         <f t="shared" si="1"/>
         <v>77.588078484968207</v>
       </c>
@@ -2460,90 +2460,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-      <c r="I27" s="13" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="I27" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="15"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16">
+      <c r="B28" s="12">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>310.04444444444454</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="I28" s="16">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="I28" s="12">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>55.173744700421707</v>
       </c>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="18"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="14"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="13" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
-      <c r="I29" s="13" t="s">
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="I29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="14"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="13" t="s">
+      <c r="J29" s="16"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="14"/>
-      <c r="N29" s="15"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16">
+      <c r="B30" s="12">
         <f>O10</f>
         <v>304</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="16">
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="12">
         <f>B28-B30</f>
         <v>6.0444444444445367</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="I30" s="16">
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="I30" s="12">
         <f>P10</f>
         <v>54.098109769335629</v>
       </c>
-      <c r="J30" s="17"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="16">
+      <c r="J30" s="13"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="12">
         <f>I28-I30</f>
         <v>1.0756349310860784</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="18"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2588,24 +2588,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="18"/>
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
@@ -2795,44 +2795,44 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
-        <v>0</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12" t="s">
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
         <v>9</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>30</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>34</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <v>10</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>19</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <v>12</v>
       </c>
-      <c r="M9" s="11">
-        <v>0</v>
-      </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11">
+      <c r="M9" s="10">
+        <v>0</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10">
         <f t="shared" si="0"/>
         <v>114</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="10">
         <f t="shared" si="1"/>
         <v>54.575222848826634</v>
       </c>
@@ -3093,90 +3093,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-      <c r="I27" s="13" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="I27" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="15"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16">
+      <c r="B28" s="12">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>75.73333333333332</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="I28" s="16">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="I28" s="12">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>36.255820559220467</v>
       </c>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="18"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="14"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="13" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
-      <c r="I29" s="13" t="s">
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="I29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="14"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="13" t="s">
+      <c r="J29" s="16"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="14"/>
-      <c r="N29" s="15"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16">
+      <c r="B30" s="12">
         <f>O10</f>
         <v>78</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="16">
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="12">
         <f>B28-B30</f>
         <v>-2.2666666666666799</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="I30" s="16">
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="I30" s="12">
         <f>P10</f>
         <v>37.340941949197173</v>
       </c>
-      <c r="J30" s="17"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="16">
+      <c r="J30" s="13"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="12">
         <f>I28-I30</f>
         <v>-1.085121389976706</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="18"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3221,24 +3221,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="18"/>
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
@@ -3428,44 +3428,44 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
-        <v>0</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12" t="s">
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
         <v>8</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>29</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>17</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <v>17</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>7</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <v>17</v>
       </c>
-      <c r="M9" s="11">
-        <v>0</v>
-      </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11">
+      <c r="M9" s="10">
+        <v>0</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="10">
         <f t="shared" si="1"/>
         <v>34.923645881583106</v>
       </c>
@@ -3726,90 +3726,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-      <c r="I27" s="13" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="I27" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="15"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16">
+      <c r="B28" s="12">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>32.711111111111109</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="I28" s="16">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="I28" s="12">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>12.025171166711198</v>
       </c>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="18"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="14"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="13" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
-      <c r="I29" s="13" t="s">
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="I29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="14"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="13" t="s">
+      <c r="J29" s="16"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="14"/>
-      <c r="N29" s="15"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16">
+      <c r="B30" s="12">
         <f>O10</f>
         <v>52</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="16">
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="12">
         <f>B28-B30</f>
         <v>-19.288888888888891</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="I30" s="16">
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="I30" s="12">
         <f>P10</f>
         <v>19.116100903603385</v>
       </c>
-      <c r="J30" s="17"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="16">
+      <c r="J30" s="13"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="12">
         <f>I28-I30</f>
         <v>-7.0909297368921873</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="18"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3837,7 +3837,7 @@
   <dimension ref="A2:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="E30" sqref="E30:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3854,24 +3854,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="18"/>
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
@@ -4061,44 +4061,44 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
-        <v>0</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12" t="s">
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
         <v>64</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>89</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>122</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <v>70</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>50</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <v>20</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="10">
         <v>25</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11">
+      <c r="N9" s="10"/>
+      <c r="O9" s="10">
         <f t="shared" si="0"/>
         <v>440</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="10">
         <f t="shared" si="1"/>
         <v>42.63565891472868</v>
       </c>
@@ -4359,90 +4359,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-      <c r="I27" s="13" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="I27" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="15"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16">
+      <c r="B28" s="12">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>443.02222222222224</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="I28" s="16">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="I28" s="12">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>42.928509905254074</v>
       </c>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="18"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="14"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="13" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
-      <c r="I29" s="13" t="s">
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="I29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="14"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="13" t="s">
+      <c r="J29" s="16"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="14"/>
-      <c r="N29" s="15"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16">
+      <c r="B30" s="12">
         <f>O10</f>
         <v>288</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="16">
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="12">
         <f>B28-B30</f>
         <v>155.02222222222224</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="I30" s="16">
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="I30" s="12">
         <f>P10</f>
         <v>27.906976744186046</v>
       </c>
-      <c r="J30" s="17"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="16">
+      <c r="J30" s="13"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="12">
         <f>I28-I30</f>
         <v>15.021533161068028</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="18"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -4487,24 +4487,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="18"/>
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
@@ -4694,44 +4694,44 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
-        <v>0</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12" t="s">
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
         <v>18</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>19</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="10">
         <v>21</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <v>10</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>26</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <v>20</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="10">
         <v>4</v>
       </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11">
+      <c r="N9" s="10"/>
+      <c r="O9" s="10">
         <f t="shared" si="0"/>
         <v>118</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="10">
         <f t="shared" si="1"/>
         <v>20.998608397307905</v>
       </c>
@@ -4992,90 +4992,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-      <c r="I27" s="13" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="I27" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="15"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16">
+      <c r="B28" s="12">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>54.222222222222229</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="I28" s="16">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="I28" s="12">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>9.649078058273318</v>
       </c>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="18"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="14"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="13" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
-      <c r="I29" s="13" t="s">
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="I29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="14"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="13" t="s">
+      <c r="J29" s="16"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="14"/>
-      <c r="N29" s="15"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16">
+      <c r="B30" s="12">
         <f>O10</f>
         <v>37</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="16">
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="12">
         <f>B28-B30</f>
         <v>17.222222222222229</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="I30" s="16">
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="I30" s="12">
         <f>P10</f>
         <v>6.5843094127151911</v>
       </c>
-      <c r="J30" s="17"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="16">
+      <c r="J30" s="13"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="12">
         <f>I28-I30</f>
         <v>3.0647686455581269</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="18"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -5103,7 +5103,7 @@
   <dimension ref="A2:P30"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+      <selection activeCell="E30" sqref="E30:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5120,24 +5120,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="18"/>
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
@@ -5327,44 +5327,44 @@
       </c>
     </row>
     <row r="9" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
-        <v>0</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12" t="s">
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
         <v>2</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="10">
         <v>2</v>
       </c>
-      <c r="I9" s="11">
-        <v>0</v>
-      </c>
-      <c r="J9" s="11">
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10">
         <v>1</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>1</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <v>2</v>
       </c>
-      <c r="M9" s="11">
-        <v>0</v>
-      </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11">
+      <c r="M9" s="10">
+        <v>0</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="10">
         <f t="shared" si="1"/>
         <v>3.8298401999176588</v>
       </c>
@@ -5625,90 +5625,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="15"/>
-      <c r="I27" s="13" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="I27" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="15"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="17"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16">
+      <c r="B28" s="12">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>8.1777777777777789</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="I28" s="16">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="I28" s="12">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>3.9149477599158242</v>
       </c>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="18"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="14"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="13" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="15"/>
-      <c r="I29" s="13" t="s">
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="I29" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="14"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="13" t="s">
+      <c r="J29" s="16"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="14"/>
-      <c r="N29" s="15"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="17"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16">
+      <c r="B30" s="12">
         <f>O10</f>
         <v>8</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="16">
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="12">
         <f>B28-B30</f>
         <v>0.17777777777777892</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="I30" s="16">
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="I30" s="12">
         <f>P10</f>
         <v>3.8298401999176588</v>
       </c>
-      <c r="J30" s="17"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="16">
+      <c r="J30" s="13"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="12">
         <f>I28-I30</f>
         <v>8.5107559998165438E-2</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="18"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
Prognose, zwischenergebnis. Callback Problematik
</commit_message>
<xml_diff>
--- a/docs/PrognoseCalc/PrognoseCalc-ABSCalc.xlsx
+++ b/docs/PrognoseCalc/PrognoseCalc-ABSCalc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\thoma\IdeaProjects\GDWWS2021GeraschSalamonSchumann\docs\PrognoseCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB19689-ECCE-4DE6-BB86-224804856500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920DDE7D-144A-4897-8946-616A68DB2908}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29580" yWindow="1215" windowWidth="27450" windowHeight="18840" tabRatio="857" activeTab="5" xr2:uid="{6A5BFC6A-5A01-4EA7-8DAE-9EDEA8B95B90}"/>
+    <workbookView xWindow="-33090" yWindow="1590" windowWidth="27450" windowHeight="18840" tabRatio="857" xr2:uid="{6A5BFC6A-5A01-4EA7-8DAE-9EDEA8B95B90}"/>
   </bookViews>
   <sheets>
     <sheet name="05374-OBK2021" sheetId="1" r:id="rId1"/>
@@ -331,6 +331,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -347,9 +350,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E867732-46F2-41F1-B375-A76F3F3987BC}">
   <dimension ref="A2:V30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:G30"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,24 +686,24 @@
       </c>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="12"/>
       <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1191,90 +1191,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="I27" s="15" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="I27" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="12">
+      <c r="B28" s="13">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>131.91111111111113</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-      <c r="I28" s="12">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+      <c r="I28" s="13">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>48.492809813585417</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="15"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="15" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-      <c r="I29" s="15" t="s">
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="I29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="15" t="s">
+      <c r="J29" s="17"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="16"/>
-      <c r="N29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="18"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="12">
+      <c r="B30" s="13">
         <f>O10</f>
         <v>128</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="12">
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="13">
         <f>B28-B30</f>
         <v>3.9111111111111256</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="I30" s="12">
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
+      <c r="I30" s="13">
         <f>P10</f>
         <v>47.055017608869875</v>
       </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="12">
+      <c r="J30" s="14"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="13">
         <f>I28-I30</f>
         <v>1.4377922047155423</v>
       </c>
-      <c r="M30" s="13"/>
-      <c r="N30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1321,24 +1321,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="12"/>
       <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1826,90 +1826,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="I27" s="15" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="I27" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="12">
+      <c r="B28" s="13">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>48.533333333333339</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-      <c r="I28" s="12">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+      <c r="I28" s="13">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>4.7028423772609891</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="15"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="15" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-      <c r="I29" s="15" t="s">
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="I29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="15" t="s">
+      <c r="J29" s="17"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="16"/>
-      <c r="N29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="18"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="12">
+      <c r="B30" s="13">
         <f>O10</f>
         <v>122</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="12">
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="13">
         <f>B28-B30</f>
         <v>-73.466666666666669</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="I30" s="12">
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
+      <c r="I30" s="13">
         <f>P10</f>
         <v>11.821705426356589</v>
       </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="12">
+      <c r="J30" s="14"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="13">
         <f>I28-I30</f>
         <v>-7.1188630490955997</v>
       </c>
-      <c r="M30" s="13"/>
-      <c r="N30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1938,7 +1938,7 @@
   <dimension ref="A2:P30"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,24 +1955,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="12"/>
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
@@ -2460,90 +2460,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="I27" s="15" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="I27" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="12">
+      <c r="B28" s="13">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>310.04444444444454</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-      <c r="I28" s="12">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+      <c r="I28" s="13">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>55.173744700421707</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="15"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="15" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-      <c r="I29" s="15" t="s">
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="I29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="15" t="s">
+      <c r="J29" s="17"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="16"/>
-      <c r="N29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="18"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="12">
+      <c r="B30" s="13">
         <f>O10</f>
         <v>304</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="12">
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="13">
         <f>B28-B30</f>
         <v>6.0444444444445367</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="I30" s="12">
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
+      <c r="I30" s="13">
         <f>P10</f>
         <v>54.098109769335629</v>
       </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="12">
+      <c r="J30" s="14"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="13">
         <f>I28-I30</f>
         <v>1.0756349310860784</v>
       </c>
-      <c r="M30" s="13"/>
-      <c r="N30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -2588,24 +2588,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="12"/>
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
@@ -3093,90 +3093,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="I27" s="15" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="I27" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="12">
+      <c r="B28" s="13">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>75.73333333333332</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-      <c r="I28" s="12">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+      <c r="I28" s="13">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>36.255820559220467</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="15"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="15" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-      <c r="I29" s="15" t="s">
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="I29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="15" t="s">
+      <c r="J29" s="17"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="16"/>
-      <c r="N29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="18"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="12">
+      <c r="B30" s="13">
         <f>O10</f>
         <v>78</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="12">
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="13">
         <f>B28-B30</f>
         <v>-2.2666666666666799</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="I30" s="12">
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
+      <c r="I30" s="13">
         <f>P10</f>
         <v>37.340941949197173</v>
       </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="12">
+      <c r="J30" s="14"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="13">
         <f>I28-I30</f>
         <v>-1.085121389976706</v>
       </c>
-      <c r="M30" s="13"/>
-      <c r="N30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3204,7 +3204,7 @@
   <dimension ref="A2:P30"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3221,24 +3221,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="12"/>
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
@@ -3726,90 +3726,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="I27" s="15" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="I27" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="12">
+      <c r="B28" s="13">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>32.711111111111109</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-      <c r="I28" s="12">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+      <c r="I28" s="13">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>12.025171166711198</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="15"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="15" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-      <c r="I29" s="15" t="s">
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="I29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="15" t="s">
+      <c r="J29" s="17"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="16"/>
-      <c r="N29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="18"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="12">
+      <c r="B30" s="13">
         <f>O10</f>
         <v>52</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="12">
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="13">
         <f>B28-B30</f>
         <v>-19.288888888888891</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="I30" s="12">
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
+      <c r="I30" s="13">
         <f>P10</f>
         <v>19.116100903603385</v>
       </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="12">
+      <c r="J30" s="14"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="13">
         <f>I28-I30</f>
         <v>-7.0909297368921873</v>
       </c>
-      <c r="M30" s="13"/>
-      <c r="N30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3836,8 +3836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5599083B-8C9C-4F78-80B8-30E6C05390A7}">
   <dimension ref="A2:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:G30"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3854,24 +3854,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="12"/>
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
@@ -4359,90 +4359,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="I27" s="15" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="I27" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="12">
+      <c r="B28" s="13">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>443.02222222222224</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-      <c r="I28" s="12">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+      <c r="I28" s="13">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>42.928509905254074</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="15"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="15" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-      <c r="I29" s="15" t="s">
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="I29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="15" t="s">
+      <c r="J29" s="17"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="16"/>
-      <c r="N29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="18"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="12">
+      <c r="B30" s="13">
         <f>O10</f>
         <v>288</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="12">
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="13">
         <f>B28-B30</f>
         <v>155.02222222222224</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="I30" s="12">
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
+      <c r="I30" s="13">
         <f>P10</f>
         <v>27.906976744186046</v>
       </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="12">
+      <c r="J30" s="14"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="13">
         <f>I28-I30</f>
         <v>15.021533161068028</v>
       </c>
-      <c r="M30" s="13"/>
-      <c r="N30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -4487,24 +4487,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="12"/>
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
@@ -4992,90 +4992,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="I27" s="15" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="I27" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="12">
+      <c r="B28" s="13">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>54.222222222222229</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-      <c r="I28" s="12">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+      <c r="I28" s="13">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>9.649078058273318</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="15"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="15" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-      <c r="I29" s="15" t="s">
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="I29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="15" t="s">
+      <c r="J29" s="17"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="16"/>
-      <c r="N29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="18"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="12">
+      <c r="B30" s="13">
         <f>O10</f>
         <v>37</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="12">
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="13">
         <f>B28-B30</f>
         <v>17.222222222222229</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="I30" s="12">
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
+      <c r="I30" s="13">
         <f>P10</f>
         <v>6.5843094127151911</v>
       </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="12">
+      <c r="J30" s="14"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="13">
         <f>I28-I30</f>
         <v>3.0647686455581269</v>
       </c>
-      <c r="M30" s="13"/>
-      <c r="N30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -5120,24 +5120,24 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="18"/>
+      <c r="E4" s="12"/>
       <c r="G4" s="4" t="s">
         <v>18</v>
       </c>
@@ -5625,90 +5625,90 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="I27" s="15" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="I27" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="12">
+      <c r="B28" s="13">
         <f>ABS(IF(E24&lt;=0,G21,F21))</f>
         <v>8.1777777777777789</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
-      <c r="I28" s="12">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+      <c r="I28" s="13">
         <f>ABS(IF(L24&lt;=0,N21,M21))</f>
         <v>3.9149477599158242</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="15"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="15" t="s">
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-      <c r="I29" s="15" t="s">
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="I29" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="15" t="s">
+      <c r="J29" s="17"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="M29" s="16"/>
-      <c r="N29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="18"/>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="12">
+      <c r="B30" s="13">
         <f>O10</f>
         <v>8</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="12">
+      <c r="C30" s="14"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="13">
         <f>B28-B30</f>
         <v>0.17777777777777892</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
-      <c r="I30" s="12">
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
+      <c r="I30" s="13">
         <f>P10</f>
         <v>3.8298401999176588</v>
       </c>
-      <c r="J30" s="13"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="12">
+      <c r="J30" s="14"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="13">
         <f>I28-I30</f>
         <v>8.5107559998165438E-2</v>
       </c>
-      <c r="M30" s="13"/>
-      <c r="N30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>